<commit_message>
add error message pop-ups to 2_add_layouts/app.R
</commit_message>
<xml_diff>
--- a/dsfworld6_script_workflows.xlsx
+++ b/dsfworld6_script_workflows.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Input</t>
   </si>
@@ -41,6 +41,9 @@
     <t>raw RFU user data</t>
   </si>
   <si>
+    <t>formatted data</t>
+  </si>
+  <si>
     <t>Tmas from model fitting</t>
   </si>
   <si>
@@ -63,6 +66,21 @@
   </si>
   <si>
     <t>upload_formatters.R</t>
+  </si>
+  <si>
+    <t>formatted data (nested by each input data column)</t>
+  </si>
+  <si>
+    <t>merge_layouts app.R</t>
+  </si>
+  <si>
+    <t>Addressed</t>
+  </si>
+  <si>
+    <t>Differences in raw data upload formats</t>
+  </si>
+  <si>
+    <t>labeled data</t>
   </si>
 </sst>
 </file>
@@ -377,69 +395,85 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="22" customWidth="1"/>
-    <col min="2" max="3" width="19.6640625" customWidth="1"/>
-    <col min="4" max="4" width="23.83203125" customWidth="1"/>
+    <col min="2" max="2" width="20.83203125" customWidth="1"/>
+    <col min="3" max="3" width="21.6640625" customWidth="1"/>
+    <col min="4" max="4" width="34" customWidth="1"/>
+    <col min="5" max="5" width="44.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
       <c r="D1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
reanmed plotting/app.R to plot/app.R
</commit_message>
<xml_diff>
--- a/dsfworld6_script_workflows.xlsx
+++ b/dsfworld6_script_workflows.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="500"/>
+    <workbookView xWindow="25600" yWindow="460" windowWidth="38400" windowHeight="21140" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Input</t>
   </si>
@@ -35,60 +35,98 @@
     <t>Script</t>
   </si>
   <si>
-    <t>Output</t>
-  </si>
-  <si>
-    <t>raw RFU user data</t>
-  </si>
-  <si>
-    <t>formatted data</t>
-  </si>
-  <si>
-    <t>Tmas from model fitting</t>
-  </si>
-  <si>
-    <t>Tmas from dRFU</t>
-  </si>
-  <si>
-    <t>layout file</t>
-  </si>
-  <si>
-    <t xml:space="preserve">formatted layout </t>
-  </si>
-  <si>
-    <t>nested formatted data</t>
-  </si>
-  <si>
     <t>Standalone app</t>
   </si>
   <si>
-    <t>upload_raw app.R</t>
-  </si>
-  <si>
     <t>upload_formatters.R</t>
   </si>
   <si>
     <t>formatted data (nested by each input data column)</t>
   </si>
   <si>
-    <t>merge_layouts app.R</t>
-  </si>
-  <si>
-    <t>Addressed</t>
-  </si>
-  <si>
     <t>Differences in raw data upload formats</t>
   </si>
   <si>
-    <t>labeled data</t>
+    <t>1_upload_raw/app.R</t>
+  </si>
+  <si>
+    <t>2_add_layouts/app.R</t>
+  </si>
+  <si>
+    <t>3_plot/app.R</t>
+  </si>
+  <si>
+    <t>layout_handling.R</t>
+  </si>
+  <si>
+    <t>plotting.R</t>
+  </si>
+  <si>
+    <t>formatted data (values$df_1)</t>
+  </si>
+  <si>
+    <t>raw RFU user data (a csv)</t>
+  </si>
+  <si>
+    <t>Issues addressed</t>
+  </si>
+  <si>
+    <t>Efficient, user-friendly mapping of multi-variable layouts to data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">formatted data, with arbitrary number of user-defined layout variables as columns </t>
+  </si>
+  <si>
+    <t>values$df</t>
+  </si>
+  <si>
+    <t>formatted data, with or without layout (values$df)</t>
+  </si>
+  <si>
+    <t>Flexible creation of information-rich plots, based on input variables</t>
+  </si>
+  <si>
+    <t>user-made plots, with customizable text sizes</t>
+  </si>
+  <si>
+    <t>plot_updated()</t>
+  </si>
+  <si>
+    <t>Primary output</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Primary output object names </t>
+  </si>
+  <si>
+    <t>Minor (internal use) outputs</t>
+  </si>
+  <si>
+    <t>values$df_1</t>
+  </si>
+  <si>
+    <t>values$data_raw</t>
+  </si>
+  <si>
+    <t>values$layout</t>
+  </si>
+  <si>
+    <t>plot_initial(), height, values$chosen_plot</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -116,8 +154,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -395,85 +440,113 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22" customWidth="1"/>
-    <col min="2" max="2" width="20.83203125" customWidth="1"/>
-    <col min="3" max="3" width="21.6640625" customWidth="1"/>
-    <col min="4" max="4" width="34" customWidth="1"/>
-    <col min="5" max="5" width="44.5" customWidth="1"/>
+    <col min="1" max="1" width="17.83203125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="19.33203125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="21.6640625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="34.1640625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="25.83203125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="26.1640625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="28.6640625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="E4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E8" t="s">
-        <v>8</v>
+      <c r="D4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
before starting on monday
</commit_message>
<xml_diff>
--- a/dsfworld6_script_workflows.xlsx
+++ b/dsfworld6_script_workflows.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="25600" yWindow="460" windowWidth="38400" windowHeight="21140" tabRatio="500"/>
+    <workbookView xWindow="1200" yWindow="6180" windowWidth="14400" windowHeight="9660" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -443,7 +443,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
4_analyze/app.R with downloading of plots and tmas
</commit_message>
<xml_diff>
--- a/dsfworld6_script_workflows.xlsx
+++ b/dsfworld6_script_workflows.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1200" yWindow="6180" windowWidth="14400" windowHeight="9660" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
   <si>
     <t>Input</t>
   </si>
@@ -111,6 +111,21 @@
   </si>
   <si>
     <t>plot_initial(), height, values$chosen_plot</t>
+  </si>
+  <si>
+    <t>4_analyze/app.R</t>
+  </si>
+  <si>
+    <t>Robust dRFU and curve fitting analysis by multiple possible fitting models</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tmas for input data, and sigmoid fits </t>
+  </si>
+  <si>
+    <t>analysis.R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">values$tm_table_dRFU, values$df_models, values$df_tm_models, values$df_BIC_display </t>
   </si>
 </sst>
 </file>
@@ -440,15 +455,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="A10" sqref="A10:XFD15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.83203125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="44.1640625" style="3" customWidth="1"/>
     <col min="2" max="2" width="19.33203125" style="3" customWidth="1"/>
     <col min="3" max="3" width="21.6640625" style="3" customWidth="1"/>
     <col min="4" max="4" width="34.1640625" style="3" customWidth="1"/>
@@ -503,7 +518,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>11</v>
       </c>
@@ -526,7 +541,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>17</v>
       </c>
@@ -547,6 +562,26 @@
       </c>
       <c r="G4" s="3" t="s">
         <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="64" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
combined_modules/app.R fully working GUI, server implemented through modeling and uploads
</commit_message>
<xml_diff>
--- a/dsfworld6_script_workflows.xlsx
+++ b/dsfworld6_script_workflows.xlsx
@@ -9,10 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="500"/>
+    <workbookView xWindow="25600" yWindow="460" windowWidth="19200" windowHeight="21140" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="For downloads " sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="108">
   <si>
     <t>Input</t>
   </si>
@@ -126,6 +129,231 @@
   </si>
   <si>
     <t xml:space="preserve">values$tm_table_dRFU, values$df_models, values$df_tm_models, values$df_BIC_display </t>
+  </si>
+  <si>
+    <t>object</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Section</t>
+  </si>
+  <si>
+    <t>Tma by dRFU</t>
+  </si>
+  <si>
+    <t>Tma by best fit</t>
+  </si>
+  <si>
+    <t>Replicate-averaged raw data</t>
+  </si>
+  <si>
+    <t>Data with fits</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>done</t>
+  </si>
+  <si>
+    <t>quick</t>
+  </si>
+  <si>
+    <t>Tma by dRFU, no replicate averaging</t>
+  </si>
+  <si>
+    <t>Tma by fit, no replicate averaging</t>
+  </si>
+  <si>
+    <t>Reformatted raw data</t>
+  </si>
+  <si>
+    <t>supp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Normalized raw data </t>
+  </si>
+  <si>
+    <t>Raw data, dRFU</t>
+  </si>
+  <si>
+    <t>win3d</t>
+  </si>
+  <si>
+    <t>n2r</t>
+  </si>
+  <si>
+    <t>values$sX_X_list, all</t>
+  </si>
+  <si>
+    <t>values$df_models</t>
+  </si>
+  <si>
+    <t>values$df_tm_models</t>
+  </si>
+  <si>
+    <t>values$df_BIC_models</t>
+  </si>
+  <si>
+    <t>raw data</t>
+  </si>
+  <si>
+    <t>fit results</t>
+  </si>
+  <si>
+    <t>rmds</t>
+  </si>
+  <si>
+    <t>tma_by_dRFU()</t>
+  </si>
+  <si>
+    <t>in values$df</t>
+  </si>
+  <si>
+    <t>in values$df_models</t>
+  </si>
+  <si>
+    <t>s1_list</t>
+  </si>
+  <si>
+    <t>model</t>
+  </si>
+  <si>
+    <t>df_BIC</t>
+  </si>
+  <si>
+    <t>df_models</t>
+  </si>
+  <si>
+    <t>tm_table_models</t>
+  </si>
+  <si>
+    <t>tm_models_all</t>
+  </si>
+  <si>
+    <t>df_models_sgd1</t>
+  </si>
+  <si>
+    <t>row_</t>
+  </si>
+  <si>
+    <t>col_</t>
+  </si>
+  <si>
+    <t>well_</t>
+  </si>
+  <si>
+    <t>well_f_</t>
+  </si>
+  <si>
+    <t>well</t>
+  </si>
+  <si>
+    <t>condition</t>
+  </si>
+  <si>
+    <t>[condition</t>
+  </si>
+  <si>
+    <t>elements]</t>
+  </si>
+  <si>
+    <t>data</t>
+  </si>
+  <si>
+    <t>sgd1</t>
+  </si>
+  <si>
+    <t>peaks</t>
+  </si>
+  <si>
+    <t>model_pars</t>
+  </si>
+  <si>
+    <t>xmid_start</t>
+  </si>
+  <si>
+    <t>broom_aug</t>
+  </si>
+  <si>
+    <t>resids</t>
+  </si>
+  <si>
+    <t>predictions</t>
+  </si>
+  <si>
+    <t>glance</t>
+  </si>
+  <si>
+    <t>BIC</t>
+  </si>
+  <si>
+    <t>which_model</t>
+  </si>
+  <si>
+    <t>Temperature</t>
+  </si>
+  <si>
+    <t>Temperature_norm</t>
+  </si>
+  <si>
+    <t>pred</t>
+  </si>
+  <si>
+    <t>value_norm</t>
+  </si>
+  <si>
+    <t>component</t>
+  </si>
+  <si>
+    <t>mean_tma1</t>
+  </si>
+  <si>
+    <t>sd_tma1</t>
+  </si>
+  <si>
+    <t>mean_tma2</t>
+  </si>
+  <si>
+    <t>sd_tma2</t>
+  </si>
+  <si>
+    <t>sigmoid_1</t>
+  </si>
+  <si>
+    <t>sigmoid_2</t>
+  </si>
+  <si>
+    <t>tma</t>
+  </si>
+  <si>
+    <t>row of data, in A format</t>
+  </si>
+  <si>
+    <t>col of data</t>
+  </si>
+  <si>
+    <t>well of data, in "A1" format</t>
+  </si>
+  <si>
+    <t>well of data, as an ordered factor</t>
+  </si>
+  <si>
+    <t>well, as in the uploaded data</t>
+  </si>
+  <si>
+    <t>experimental condition in that well</t>
+  </si>
+  <si>
+    <t>all individual experiment variables</t>
+  </si>
+  <si>
+    <t>nested dataframe, one for each well, with row_, col_, well_, well_f_, well, condition, [condition elements], Temperature, value, mean, sd, Temperature_norm, value_norm, mean_norm, sd_norm, and the following nested dataframes:</t>
+  </si>
+  <si>
+    <t>sgd1, peaks, model, model_pars, xmid_start, broom_aug, resids, predictions, glance</t>
   </si>
 </sst>
 </file>
@@ -457,8 +685,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:XFD15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -587,4 +815,893 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D19"/>
+  <sheetViews>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="35.6640625" customWidth="1"/>
+    <col min="2" max="2" width="20.1640625" customWidth="1"/>
+    <col min="3" max="3" width="14.1640625" customWidth="1"/>
+    <col min="4" max="4" width="23.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>47</v>
+      </c>
+      <c r="D10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>48</v>
+      </c>
+      <c r="D11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>49</v>
+      </c>
+      <c r="B13" t="s">
+        <v>49</v>
+      </c>
+      <c r="D13" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>50</v>
+      </c>
+      <c r="B14" t="s">
+        <v>50</v>
+      </c>
+      <c r="D14" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>55</v>
+      </c>
+      <c r="B15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>56</v>
+      </c>
+      <c r="B16" t="s">
+        <v>51</v>
+      </c>
+      <c r="D16" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>52</v>
+      </c>
+      <c r="D17" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>54</v>
+      </c>
+      <c r="D18" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>53</v>
+      </c>
+      <c r="D19" t="s">
+        <v>57</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:G29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="22.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E2" t="s">
+        <v>71</v>
+      </c>
+      <c r="F2" t="s">
+        <v>72</v>
+      </c>
+      <c r="G2" t="s">
+        <v>73</v>
+      </c>
+      <c r="H2" t="s">
+        <v>74</v>
+      </c>
+      <c r="I2" t="s">
+        <v>75</v>
+      </c>
+      <c r="J2" t="s">
+        <v>76</v>
+      </c>
+      <c r="K2" t="s">
+        <v>77</v>
+      </c>
+      <c r="L2" t="s">
+        <v>78</v>
+      </c>
+      <c r="M2" t="s">
+        <v>62</v>
+      </c>
+      <c r="N2" t="s">
+        <v>79</v>
+      </c>
+      <c r="O2" t="s">
+        <v>80</v>
+      </c>
+      <c r="P2" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>82</v>
+      </c>
+      <c r="R2" t="s">
+        <v>83</v>
+      </c>
+      <c r="S2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D3" t="s">
+        <v>85</v>
+      </c>
+      <c r="E3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C4" t="s">
+        <v>87</v>
+      </c>
+      <c r="D4" t="s">
+        <v>88</v>
+      </c>
+      <c r="E4" t="s">
+        <v>89</v>
+      </c>
+      <c r="F4" t="s">
+        <v>90</v>
+      </c>
+      <c r="G4" t="s">
+        <v>73</v>
+      </c>
+      <c r="H4" t="s">
+        <v>86</v>
+      </c>
+      <c r="I4" t="s">
+        <v>91</v>
+      </c>
+      <c r="J4" t="s">
+        <v>68</v>
+      </c>
+      <c r="K4" t="s">
+        <v>69</v>
+      </c>
+      <c r="L4" t="s">
+        <v>70</v>
+      </c>
+      <c r="M4" t="s">
+        <v>71</v>
+      </c>
+      <c r="N4" t="s">
+        <v>74</v>
+      </c>
+      <c r="O4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D5" t="s">
+        <v>93</v>
+      </c>
+      <c r="E5" t="s">
+        <v>94</v>
+      </c>
+      <c r="F5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>66</v>
+      </c>
+      <c r="B6" t="s">
+        <v>86</v>
+      </c>
+      <c r="C6" t="s">
+        <v>73</v>
+      </c>
+      <c r="D6" t="s">
+        <v>96</v>
+      </c>
+      <c r="E6" t="s">
+        <v>97</v>
+      </c>
+      <c r="F6" t="s">
+        <v>92</v>
+      </c>
+      <c r="G6" t="s">
+        <v>94</v>
+      </c>
+      <c r="H6" t="s">
+        <v>93</v>
+      </c>
+      <c r="I6" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B7" t="s">
+        <v>86</v>
+      </c>
+      <c r="C7" t="s">
+        <v>91</v>
+      </c>
+      <c r="D7" t="s">
+        <v>76</v>
+      </c>
+      <c r="E7" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>61</v>
+      </c>
+      <c r="B10" t="s">
+        <v>62</v>
+      </c>
+      <c r="C10" t="s">
+        <v>63</v>
+      </c>
+      <c r="D10" t="s">
+        <v>64</v>
+      </c>
+      <c r="E10" t="s">
+        <v>65</v>
+      </c>
+      <c r="F10" t="s">
+        <v>66</v>
+      </c>
+      <c r="G10" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>68</v>
+      </c>
+      <c r="C11" t="s">
+        <v>72</v>
+      </c>
+      <c r="D11" t="s">
+        <v>72</v>
+      </c>
+      <c r="E11" t="s">
+        <v>86</v>
+      </c>
+      <c r="F11" t="s">
+        <v>86</v>
+      </c>
+      <c r="G11" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>69</v>
+      </c>
+      <c r="C12" t="s">
+        <v>73</v>
+      </c>
+      <c r="D12" t="s">
+        <v>87</v>
+      </c>
+      <c r="E12" t="s">
+        <v>92</v>
+      </c>
+      <c r="F12" t="s">
+        <v>73</v>
+      </c>
+      <c r="G12" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>70</v>
+      </c>
+      <c r="C13" t="s">
+        <v>85</v>
+      </c>
+      <c r="D13" t="s">
+        <v>88</v>
+      </c>
+      <c r="E13" t="s">
+        <v>93</v>
+      </c>
+      <c r="F13" t="s">
+        <v>96</v>
+      </c>
+      <c r="G13" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>71</v>
+      </c>
+      <c r="C14" t="s">
+        <v>86</v>
+      </c>
+      <c r="D14" t="s">
+        <v>89</v>
+      </c>
+      <c r="E14" t="s">
+        <v>94</v>
+      </c>
+      <c r="F14" t="s">
+        <v>97</v>
+      </c>
+      <c r="G14" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>72</v>
+      </c>
+      <c r="D15" t="s">
+        <v>90</v>
+      </c>
+      <c r="E15" t="s">
+        <v>95</v>
+      </c>
+      <c r="F15" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>73</v>
+      </c>
+      <c r="D16" t="s">
+        <v>73</v>
+      </c>
+      <c r="F16" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>74</v>
+      </c>
+      <c r="D17" t="s">
+        <v>86</v>
+      </c>
+      <c r="F17" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>75</v>
+      </c>
+      <c r="D18" t="s">
+        <v>91</v>
+      </c>
+      <c r="F18" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>76</v>
+      </c>
+      <c r="D19" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
+        <v>77</v>
+      </c>
+      <c r="D20" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
+        <v>78</v>
+      </c>
+      <c r="D21" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B22" t="s">
+        <v>62</v>
+      </c>
+      <c r="D22" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B23" t="s">
+        <v>79</v>
+      </c>
+      <c r="D23" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B24" t="s">
+        <v>80</v>
+      </c>
+      <c r="D24" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B25" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B27" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B28" t="s">
+        <v>84</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F38" sqref="F38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="3" max="3" width="28.6640625" customWidth="1"/>
+    <col min="4" max="13" width="19.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F1" t="s">
+        <v>64</v>
+      </c>
+      <c r="H1" t="s">
+        <v>65</v>
+      </c>
+      <c r="J1" t="s">
+        <v>66</v>
+      </c>
+      <c r="L1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D2" t="s">
+        <v>72</v>
+      </c>
+      <c r="F2" t="s">
+        <v>72</v>
+      </c>
+      <c r="H2" t="s">
+        <v>86</v>
+      </c>
+      <c r="J2" t="s">
+        <v>86</v>
+      </c>
+      <c r="L2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D3" t="s">
+        <v>73</v>
+      </c>
+      <c r="F3" t="s">
+        <v>87</v>
+      </c>
+      <c r="H3" t="s">
+        <v>92</v>
+      </c>
+      <c r="J3" t="s">
+        <v>73</v>
+      </c>
+      <c r="L3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C4" t="s">
+        <v>101</v>
+      </c>
+      <c r="D4" t="s">
+        <v>85</v>
+      </c>
+      <c r="F4" t="s">
+        <v>88</v>
+      </c>
+      <c r="H4" t="s">
+        <v>93</v>
+      </c>
+      <c r="J4" t="s">
+        <v>96</v>
+      </c>
+      <c r="L4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C5" t="s">
+        <v>102</v>
+      </c>
+      <c r="D5" t="s">
+        <v>86</v>
+      </c>
+      <c r="F5" t="s">
+        <v>89</v>
+      </c>
+      <c r="H5" t="s">
+        <v>94</v>
+      </c>
+      <c r="J5" t="s">
+        <v>97</v>
+      </c>
+      <c r="L5" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C6" t="s">
+        <v>103</v>
+      </c>
+      <c r="F6" t="s">
+        <v>90</v>
+      </c>
+      <c r="H6" t="s">
+        <v>95</v>
+      </c>
+      <c r="J6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C7" t="s">
+        <v>104</v>
+      </c>
+      <c r="F7" t="s">
+        <v>73</v>
+      </c>
+      <c r="J7" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C8" t="s">
+        <v>105</v>
+      </c>
+      <c r="F8" t="s">
+        <v>86</v>
+      </c>
+      <c r="J8" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>75</v>
+      </c>
+      <c r="F9" t="s">
+        <v>91</v>
+      </c>
+      <c r="J9" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>76</v>
+      </c>
+      <c r="F10" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>77</v>
+      </c>
+      <c r="F11" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>78</v>
+      </c>
+      <c r="F12" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>62</v>
+      </c>
+      <c r="F13" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>79</v>
+      </c>
+      <c r="F14" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>80</v>
+      </c>
+      <c r="F15" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B23" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B24" t="s">
+        <v>107</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>